<commit_message>
TIAD -> max colums in row
</commit_message>
<xml_diff>
--- a/TIAD/zad1/test.xlsx
+++ b/TIAD/zad1/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janek\Desktop\studia\sem6\Semestr6\TIAD\zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF933A6-7866-4E18-8223-96B9BF4E916A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B9CE6E-D4DE-49B4-BB92-32EC07D1BC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD9AA642-32CD-4E61-A4C1-2A9D41414023}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{AD9AA642-32CD-4E61-A4C1-2A9D41414023}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,30 +36,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>XDD</t>
-  </si>
-  <si>
-    <t>ddd</t>
-  </si>
-  <si>
-    <t>ass</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>halo</t>
-  </si>
-  <si>
-    <t>puste</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+  <si>
+    <t>jeden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dwa </t>
+  </si>
+  <si>
+    <t>trzy</t>
+  </si>
+  <si>
+    <t>XD2</t>
+  </si>
+  <si>
+    <t>XD3</t>
+  </si>
+  <si>
+    <t>cztery</t>
+  </si>
+  <si>
+    <t>piec</t>
+  </si>
+  <si>
+    <t>szesc</t>
+  </si>
+  <si>
+    <t>siedem</t>
+  </si>
+  <si>
+    <t>Title1</t>
+  </si>
+  <si>
+    <t>Title2</t>
+  </si>
+  <si>
+    <t>title3</t>
+  </si>
+  <si>
+    <t>title4</t>
+  </si>
+  <si>
+    <t>title5</t>
+  </si>
+  <si>
+    <t>title6</t>
+  </si>
+  <si>
+    <t>title7</t>
+  </si>
+  <si>
+    <t>Długi tekst, długi tekst, długi tekst Długi tekst, długi tekst, długi tekst</t>
   </si>
 </sst>
 </file>
@@ -432,67 +459,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7A8354-81AC-434C-ABCE-F9E973CF73BB}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
+      <c r="G3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TIAD -> fixed sizing in docx and preview in gui
</commit_message>
<xml_diff>
--- a/TIAD/zad1/test.xlsx
+++ b/TIAD/zad1/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janek\Desktop\studia\sem6\Semestr6\TIAD\zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B9CE6E-D4DE-49B4-BB92-32EC07D1BC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0295E5A5-70C5-404E-9212-DE281D4DFE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{AD9AA642-32CD-4E61-A4C1-2A9D41414023}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TIAD -> fixed convert to pdf
</commit_message>
<xml_diff>
--- a/TIAD/zad1/test.xlsx
+++ b/TIAD/zad1/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janek\Desktop\studia\sem6\Semestr6\TIAD\zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0295E5A5-70C5-404E-9212-DE281D4DFE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8692E26-609F-485F-A25F-F9B7C30005D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{AD9AA642-32CD-4E61-A4C1-2A9D41414023}"/>
   </bookViews>
@@ -36,26 +36,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
-  <si>
-    <t>jeden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dwa </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>cztery</t>
+  </si>
+  <si>
+    <t>title4</t>
+  </si>
+  <si>
+    <t>Długi tekst, długi tekst, długi tekst Długi tekst, długi tekst, długi tekst</t>
+  </si>
+  <si>
+    <t>title1</t>
+  </si>
+  <si>
+    <t>title2</t>
+  </si>
+  <si>
+    <t>title3</t>
+  </si>
+  <si>
+    <t>title7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jeden </t>
+  </si>
+  <si>
+    <t>dwa</t>
   </si>
   <si>
     <t>trzy</t>
   </si>
   <si>
-    <t>XD2</t>
-  </si>
-  <si>
-    <t>XD3</t>
-  </si>
-  <si>
-    <t>cztery</t>
-  </si>
-  <si>
     <t>piec</t>
   </si>
   <si>
@@ -65,28 +77,19 @@
     <t>siedem</t>
   </si>
   <si>
-    <t>Title1</t>
-  </si>
-  <si>
-    <t>Title2</t>
-  </si>
-  <si>
-    <t>title3</t>
-  </si>
-  <si>
-    <t>title4</t>
-  </si>
-  <si>
-    <t>title5</t>
-  </si>
-  <si>
-    <t>title6</t>
-  </si>
-  <si>
-    <t>title7</t>
-  </si>
-  <si>
-    <t>Długi tekst, długi tekst, długi tekst Długi tekst, długi tekst, długi tekst</t>
+    <t>sdsada</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>XD</t>
+  </si>
+  <si>
+    <t>trele</t>
+  </si>
+  <si>
+    <t>morele</t>
   </si>
 </sst>
 </file>
@@ -462,75 +465,69 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G4"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
+      <c r="G2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TIAD -> fixes part1
</commit_message>
<xml_diff>
--- a/TIAD/zad1/test.xlsx
+++ b/TIAD/zad1/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janek\Desktop\studia\sem6\Semestr6\TIAD\zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8692E26-609F-485F-A25F-F9B7C30005D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC551824-32BD-4309-A01E-38DF42459D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{AD9AA642-32CD-4E61-A4C1-2A9D41414023}"/>
+    <workbookView xWindow="-24465" yWindow="2190" windowWidth="21600" windowHeight="11295" xr2:uid="{AD9AA642-32CD-4E61-A4C1-2A9D41414023}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -462,71 +462,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7A8354-81AC-434C-ABCE-F9E973CF73BB}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="D4:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I5" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G6" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H6" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I6" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J6" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TIAD -> converter finished
</commit_message>
<xml_diff>
--- a/TIAD/zad1/test.xlsx
+++ b/TIAD/zad1/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janek\Desktop\studia\sem6\Semestr6\TIAD\zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC551824-32BD-4309-A01E-38DF42459D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB97B5E9-8B57-49F6-B409-DA98BA1101B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24465" yWindow="2190" windowWidth="21600" windowHeight="11295" xr2:uid="{AD9AA642-32CD-4E61-A4C1-2A9D41414023}"/>
+    <workbookView xWindow="6285" yWindow="2205" windowWidth="21600" windowHeight="11295" xr2:uid="{AD9AA642-32CD-4E61-A4C1-2A9D41414023}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <dimension ref="D4:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:J6"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
tiad -> receiving words from audio without repeats
</commit_message>
<xml_diff>
--- a/TIAD/zad1/test.xlsx
+++ b/TIAD/zad1/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janek\Desktop\studia\sem6\Semestr6\TIAD\zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB97B5E9-8B57-49F6-B409-DA98BA1101B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D344BC39-6900-4755-9278-293A36F76797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="2205" windowWidth="21600" windowHeight="11295" xr2:uid="{AD9AA642-32CD-4E61-A4C1-2A9D41414023}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD9AA642-32CD-4E61-A4C1-2A9D41414023}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <dimension ref="D4:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>